<commit_message>
Minor update to mecanum spreadsheet
</commit_message>
<xml_diff>
--- a/Mecanum calculations.xlsx
+++ b/Mecanum calculations.xlsx
@@ -409,7 +409,7 @@
   <dimension ref="C5:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,14 +434,14 @@
         <v>8</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6">
         <f>D6*PI()/180</f>
-        <v>0</v>
+        <v>1.5707963267948966</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -479,19 +479,19 @@
       </c>
       <c r="E10">
         <f>D5*SIN(F6+(PI()/4)) + D7</f>
-        <v>0.70710678118654746</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="F10" s="2">
-        <f>E10*SQRT(2)/D18</f>
-        <v>1</v>
+        <f>E10/D18</f>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G10" s="2">
-        <f>H10*SQRT(2)/D18</f>
-        <v>1.0000000000000002</v>
+        <f>H10/D18</f>
+        <v>-1</v>
       </c>
       <c r="H10">
         <f>D5*COS(F6+(PI()/4)) - D7</f>
-        <v>0.70710678118654757</v>
+        <v>-0.70710678118654746</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>1</v>
@@ -515,19 +515,19 @@
       </c>
       <c r="E14">
         <f>D5*COS(F6+(PI()/4)) + D7</f>
-        <v>0.70710678118654757</v>
+        <v>-0.70710678118654746</v>
       </c>
       <c r="F14" s="2">
-        <f>E14*SQRT(2)/D18</f>
+        <f>E14/D18</f>
+        <v>-1</v>
+      </c>
+      <c r="G14" s="2">
+        <f>H14/D18</f>
         <v>1.0000000000000002</v>
-      </c>
-      <c r="G14" s="2">
-        <f>H14*SQRT(2)/D18</f>
-        <v>1</v>
       </c>
       <c r="H14">
         <f>D5*SIN(F6+(PI()/4)) - D7</f>
-        <v>0.70710678118654746</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>3</v>
@@ -538,8 +538,8 @@
         <v>10</v>
       </c>
       <c r="D18">
-        <f>SQRT(1+TAN(L6))</f>
-        <v>1</v>
+        <f>SQRT(1+TAN(L6))/SQRT(2)</f>
+        <v>0.70710678118654746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to mecanum spreadsheet
</commit_message>
<xml_diff>
--- a/Mecanum calculations.xlsx
+++ b/Mecanum calculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>FL</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>L1 normalization</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>angle(rad)</t>
+  </si>
+  <si>
+    <t>Robot centric</t>
+  </si>
+  <si>
+    <t>Joystick calculations</t>
+  </si>
+  <si>
+    <t>Stick speed</t>
+  </si>
+  <si>
+    <t>Stick normalization</t>
+  </si>
+  <si>
+    <t>Normalizers</t>
+  </si>
+  <si>
+    <t>Final speed</t>
   </si>
 </sst>
 </file>
@@ -406,17 +433,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:L18"/>
+  <dimension ref="C5:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -434,35 +461,35 @@
         <v>8</v>
       </c>
       <c r="D6" s="1">
-        <v>90</v>
+        <v>-10</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6">
         <f>D6*PI()/180</f>
-        <v>1.5707963267948966</v>
+        <v>-0.17453292519943295</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
       <c r="H6">
         <f>MOD(ABS(D6), 90)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
       </c>
       <c r="J6">
         <f>IF(H6&gt;45, 90-H6, H6)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
       </c>
       <c r="L6">
         <f>J6*PI()/180</f>
-        <v>0</v>
+        <v>0.17453292519943295</v>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
@@ -479,19 +506,19 @@
       </c>
       <c r="E10">
         <f>D5*SIN(F6+(PI()/4)) + D7</f>
-        <v>0.70710678118654757</v>
+        <v>0.57357643635104605</v>
       </c>
       <c r="F10" s="2">
         <f>E10/D18</f>
-        <v>1.0000000000000002</v>
+        <v>0.7478978246752167</v>
       </c>
       <c r="G10" s="2">
         <f>H10/D18</f>
-        <v>-1</v>
+        <v>1.0681087875566742</v>
       </c>
       <c r="H10">
         <f>D5*COS(F6+(PI()/4)) - D7</f>
-        <v>-0.70710678118654746</v>
+        <v>0.8191520442889918</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>1</v>
@@ -515,31 +542,116 @@
       </c>
       <c r="E14">
         <f>D5*COS(F6+(PI()/4)) + D7</f>
-        <v>-0.70710678118654746</v>
+        <v>0.8191520442889918</v>
       </c>
       <c r="F14" s="2">
         <f>E14/D18</f>
-        <v>-1</v>
+        <v>1.0681087875566742</v>
       </c>
       <c r="G14" s="2">
         <f>H14/D18</f>
-        <v>1.0000000000000002</v>
+        <v>0.7478978246752167</v>
       </c>
       <c r="H14">
         <f>D5*SIN(F6+(PI()/4)) - D7</f>
-        <v>0.70710678118654757</v>
+        <v>0.57357643635104605</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18">
         <f>SQRT(1+TAN(L6))/SQRT(2)</f>
-        <v>0.70710678118654746</v>
+        <v>0.76691817709207577</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <f>ATAN2(D21,D22)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="E23">
+        <f>DEGREES(D23)</f>
+        <v>45</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1">
+        <f>90-E23</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24">
+        <f>MOD(ABS(G23), 90)</f>
+        <v>45</v>
+      </c>
+      <c r="H24">
+        <f>IF(G24&gt;45, 90-G24, G24)</f>
+        <v>45</v>
+      </c>
+      <c r="I24">
+        <f>H24*PI()/180</f>
+        <v>0.78539816339744828</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <f>SQRT((D21 * D21) + (D22 * D22))</f>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <f>SQRT(1+TAN(I24))/SQRT(2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29">
+        <f>D25/(D26*SQRT(2))</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated spreadsheet to make calculations clearer
</commit_message>
<xml_diff>
--- a/Mecanum calculations.xlsx
+++ b/Mecanum calculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>FL</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Final speed</t>
+  </si>
+  <si>
+    <t>Mecanum calculations</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +113,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -119,19 +140,212 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:L29"/>
+  <dimension ref="C4:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,210 +662,301 @@
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
+    <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <f>D6*PI()/180</f>
-        <v>-0.17453292519943295</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <f>MOD(ABS(D6), 90)</f>
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6">
-        <f>IF(H6&gt;45, 90-H6, H6)</f>
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6">
-        <f>J6*PI()/180</f>
-        <v>0.17453292519943295</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>D5*SIN(F6+(PI()/4)) + D7</f>
-        <v>0.57357643635104605</v>
-      </c>
-      <c r="F10" s="2">
-        <f>E10/D18</f>
-        <v>0.7478978246752167</v>
-      </c>
-      <c r="G10" s="2">
-        <f>H10/D18</f>
-        <v>1.0681087875566742</v>
-      </c>
-      <c r="H10">
-        <f>D5*COS(F6+(PI()/4)) - D7</f>
-        <v>0.8191520442889918</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2">
+        <f>IF(D9 &gt; 0, ATAN2(D5,D6), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <f>DEGREES(D7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4">
+        <f>90-E7</f>
+        <v>90</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="9"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2">
+        <f>MOD(ABS(G7), 90)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <f>IF(G8&gt;45, 90-G8, G8)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <f>H8*PI()/180</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2">
+        <f>SQRT((D5 * D5) + (D6 * D6))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SQRT(1+TAN(I8))/SQRT(2)</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="9"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="12">
+        <f>D9/(D10*SQRT(2))</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="16" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="15">
+        <f>D12</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="14">
+        <f>G7</f>
+        <v>90</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="2">
+        <f>D18*PI()/180</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2">
+        <f>MOD(ABS(D18), 90)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="2">
+        <f>IF(H18&gt;45, 90-H18, H18)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="10">
+        <f>J18*PI()/180</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="25">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="12">
+        <f>SQRT(1+TAN(L18))/SQRT(2)</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13"/>
+    </row>
+    <row r="21" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D22" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="17">
+        <f>D17*SIN(F18+(PI()/4)) + D19</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="F22" s="19">
+        <f>E22/D20</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="G22" s="20">
+        <f>H22/D20</f>
+        <v>-1</v>
+      </c>
+      <c r="H22" s="18">
+        <f>D17*COS(F18+(PI()/4)) - D19</f>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E14">
-        <f>D5*COS(F6+(PI()/4)) + D7</f>
-        <v>0.8191520442889918</v>
-      </c>
-      <c r="F14" s="2">
-        <f>E14/D18</f>
-        <v>1.0681087875566742</v>
-      </c>
-      <c r="G14" s="2">
-        <f>H14/D18</f>
-        <v>0.7478978246752167</v>
-      </c>
-      <c r="H14">
-        <f>D5*SIN(F6+(PI()/4)) - D7</f>
-        <v>0.57357643635104605</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="E26" s="17">
+        <f>D17*COS(F18+(PI()/4)) + D19</f>
+        <v>-0.70710678118654746</v>
+      </c>
+      <c r="F26" s="23">
+        <f>E26/D20</f>
+        <v>-1</v>
+      </c>
+      <c r="G26" s="24">
+        <f>H26/D20</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H26" s="18">
+        <f>D17*SIN(F18+(PI()/4)) - D19</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="I26" s="16" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18">
-        <f>SQRT(1+TAN(L6))/SQRT(2)</f>
-        <v>0.76691817709207577</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23">
-        <f>ATAN2(D21,D22)</f>
-        <v>0.78539816339744828</v>
-      </c>
-      <c r="E23">
-        <f>DEGREES(D23)</f>
-        <v>45</v>
-      </c>
-      <c r="F23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="1">
-        <f>90-E23</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24">
-        <f>MOD(ABS(G23), 90)</f>
-        <v>45</v>
-      </c>
-      <c r="H24">
-        <f>IF(G24&gt;45, 90-G24, G24)</f>
-        <v>45</v>
-      </c>
-      <c r="I24">
-        <f>H24*PI()/180</f>
-        <v>0.78539816339744828</v>
-      </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25">
-        <f>SQRT((D21 * D21) + (D22 * D22))</f>
-        <v>1.4142135623730951</v>
-      </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26">
-        <f>SQRT(1+TAN(I24))/SQRT(2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29">
-        <f>D25/(D26*SQRT(2))</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>